<commit_message>
ch3 update, starting ch4, adding data .csv
</commit_message>
<xml_diff>
--- a/ch_4/data/table_4_3.xlsx
+++ b/ch_4/data/table_4_3.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="18380" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14880" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Table 4.3.  Frequency distribution of bycatch.  Data from Bartle (1991).</t>
   </si>
@@ -32,15 +33,37 @@
   <si>
     <t>Number of hauls with this level of by-catch</t>
   </si>
+  <si>
+    <t>bycatch</t>
+  </si>
+  <si>
+    <t>frequency</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -63,13 +86,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -401,8 +428,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -566,6 +593,179 @@
         <v>17</v>
       </c>
       <c r="B21">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>807</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19">
+        <v>17</v>
+      </c>
+      <c r="B19">
         <v>1</v>
       </c>
     </row>

</xml_diff>